<commit_message>
mediciones frecs bajas osciloscopio
</commit_message>
<xml_diff>
--- a/Mediciones/Bode labo electro.xlsx
+++ b/Mediciones/Bode labo electro.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomas\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rochi\Google Drive\Materias\Laboratorio de electrónica\TPs\Labo-de-Electro-tp1\Mediciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6ED1AD08-F097-44F4-AB8F-1371F613AE92}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21333" windowHeight="8247" xr2:uid="{045997C5-3368-43B8-81A4-AA60503ED603}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21330" windowHeight="8250"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +44,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -106,7 +105,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -143,7 +142,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -181,10 +180,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$29</c:f>
+              <c:f>Hoja1!$A$2:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -268,16 +267,22 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$D$2:$D$29</c:f>
+              <c:f>Hoja1!$D$2:$D$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>-1.7216833462721778E-2</c:v>
                 </c:pt>
@@ -361,6 +366,12 @@
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>-17.957174412697412</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-31.70053304058364</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-25.763855419176181</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -439,7 +450,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="511404600"/>
@@ -501,7 +512,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="511398040"/>
@@ -518,6 +529,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -525,7 +537,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -549,7 +560,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1126,10 +1137,10 @@
       <xdr:rowOff>110067</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>649724</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>147615</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>149087</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1158,7 +1169,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1453,19 +1464,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6237CB71-6DCC-49E9-9D5F-66F748C20A65}">
-  <dimension ref="A1:J30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.76171875" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1482,7 +1493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1500,7 +1511,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1518,7 +1529,7 @@
         <v>-4.5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1536,7 +1547,7 @@
         <v>-6.9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1554,7 +1565,7 @@
         <v>-11.23</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8</v>
       </c>
@@ -1572,7 +1583,7 @@
         <v>-17.82</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10</v>
       </c>
@@ -1590,7 +1601,7 @@
         <v>-21.8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>14</v>
       </c>
@@ -1608,7 +1619,7 @@
         <v>-30.43</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>17</v>
       </c>
@@ -1626,7 +1637,7 @@
         <v>-34.700000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20</v>
       </c>
@@ -1644,7 +1655,7 @@
         <v>-37.479999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>22</v>
       </c>
@@ -1662,7 +1673,7 @@
         <v>-39.18</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>23</v>
       </c>
@@ -1680,7 +1691,7 @@
         <v>-41.34</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>23.7</v>
       </c>
@@ -1691,14 +1702,14 @@
         <v>3.8</v>
       </c>
       <c r="D13">
-        <f>20*LOG(C13/B13)</f>
+        <f t="shared" ref="D13:D31" si="1">20*LOG(C13/B13)</f>
         <v>-2.8898454596795786</v>
       </c>
       <c r="E13">
         <v>-42.5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>24</v>
       </c>
@@ -1709,14 +1720,14 @@
         <v>3.77</v>
       </c>
       <c r="D14">
-        <f>20*LOG(C14/B14)</f>
+        <f t="shared" si="1"/>
         <v>-2.8763590640032799</v>
       </c>
       <c r="E14">
         <v>-44</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>24.3</v>
       </c>
@@ -1727,14 +1738,14 @@
         <v>3.75</v>
       </c>
       <c r="D15">
-        <f>20*LOG(C15/B15)</f>
+        <f t="shared" si="1"/>
         <v>-2.9390895285204039</v>
       </c>
       <c r="E15">
         <v>-43</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>24.6</v>
       </c>
@@ -1745,14 +1756,14 @@
         <v>14.12</v>
       </c>
       <c r="D16">
-        <f>20*LOG(C16/B16)</f>
+        <f t="shared" si="1"/>
         <v>-3.1575045337804353</v>
       </c>
       <c r="E16">
         <v>-44</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>25</v>
       </c>
@@ -1763,14 +1774,14 @@
         <v>14</v>
       </c>
       <c r="D17">
-        <f>20*LOG(C17/B17)</f>
+        <f t="shared" si="1"/>
         <v>-3.2316377545313735</v>
       </c>
       <c r="E17">
         <v>-45</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>25.5</v>
       </c>
@@ -1781,14 +1792,14 @@
         <v>13.9</v>
       </c>
       <c r="D18">
-        <f>20*LOG(C18/B18)</f>
+        <f t="shared" si="1"/>
         <v>-3.2939024630142324</v>
       </c>
       <c r="E18">
         <v>-45</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>26</v>
       </c>
@@ -1799,14 +1810,14 @@
         <v>13.75</v>
       </c>
       <c r="D19">
-        <f>20*LOG(C19/B19)</f>
+        <f t="shared" si="1"/>
         <v>-3.3881445047705054</v>
       </c>
       <c r="E19">
         <v>-45</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>26.5</v>
       </c>
@@ -1817,14 +1828,14 @@
         <v>13.62</v>
       </c>
       <c r="D20">
-        <f>20*LOG(C20/B20)</f>
+        <f t="shared" si="1"/>
         <v>-3.4706563165608073</v>
       </c>
       <c r="E20">
         <v>-46</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>27</v>
       </c>
@@ -1835,14 +1846,14 @@
         <v>13.33</v>
       </c>
       <c r="D21">
-        <f>20*LOG(C21/B21)</f>
+        <f t="shared" si="1"/>
         <v>-3.6575954798189509</v>
       </c>
       <c r="E21">
         <v>-48</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>28</v>
       </c>
@@ -1853,14 +1864,14 @@
         <v>13.2</v>
       </c>
       <c r="D22">
-        <f>20*LOG(C22/B22)</f>
+        <f t="shared" si="1"/>
         <v>-3.7427198439791369</v>
       </c>
       <c r="E22">
         <v>-48</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>29</v>
       </c>
@@ -1871,14 +1882,14 @@
         <v>13</v>
       </c>
       <c r="D23">
-        <f>20*LOG(C23/B23)</f>
+        <f t="shared" si="1"/>
         <v>-3.8753314219593999</v>
       </c>
       <c r="E23">
         <v>-49</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>30</v>
       </c>
@@ -1889,14 +1900,14 @@
         <v>12.35</v>
       </c>
       <c r="D24">
-        <f>20*LOG(C24/B24)</f>
+        <f t="shared" si="1"/>
         <v>-4.3208593161824442</v>
       </c>
       <c r="E24">
         <v>-49</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>40</v>
       </c>
@@ -1907,14 +1918,14 @@
         <v>10.58</v>
       </c>
       <c r="D25">
-        <f>20*LOG(C25/B25)</f>
+        <f t="shared" si="1"/>
         <v>-5.6644851141127948</v>
       </c>
       <c r="E25">
         <v>-57</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>45</v>
       </c>
@@ -1925,14 +1936,14 @@
         <v>9.75</v>
       </c>
       <c r="D26">
-        <f>20*LOG(C26/B26)</f>
+        <f t="shared" si="1"/>
         <v>-6.3741061541253972</v>
       </c>
       <c r="E26">
         <v>-60</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>50</v>
       </c>
@@ -1943,14 +1954,14 @@
         <v>9</v>
       </c>
       <c r="D27">
-        <f>20*LOG(C27/B27)</f>
+        <f t="shared" si="1"/>
         <v>-7.0693482793096374</v>
       </c>
       <c r="E27">
         <v>-62</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>100</v>
       </c>
@@ -1961,14 +1972,14 @@
         <v>4.97</v>
       </c>
       <c r="D28">
-        <f>20*LOG(C28/B28)</f>
+        <f t="shared" si="1"/>
         <v>-12.307949446448443</v>
       </c>
       <c r="E28">
         <v>-74</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>200</v>
       </c>
@@ -1979,15 +1990,49 @@
         <v>2.61</v>
       </c>
       <c r="D29">
-        <f>20*LOG(C29/B29)</f>
+        <f t="shared" si="1"/>
         <v>-17.957174412697412</v>
       </c>
       <c r="E29">
         <v>-85</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1000</v>
+      </c>
+      <c r="B30">
+        <v>20</v>
+      </c>
+      <c r="C30">
+        <v>0.52</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>-31.70053304058364</v>
+      </c>
+      <c r="E30">
+        <v>-86</v>
+      </c>
       <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>500</v>
+      </c>
+      <c r="B31">
+        <v>20</v>
+      </c>
+      <c r="C31">
+        <v>1.03</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>-25.763855419176181</v>
+      </c>
+      <c r="E31">
+        <v>-85</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ejercicio 1 listo (se podria revisar)
</commit_message>
<xml_diff>
--- a/Mediciones/Bode labo electro.xlsx
+++ b/Mediciones/Bode labo electro.xlsx
@@ -1467,8 +1467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2031,7 +2031,7 @@
         <v>-25.763855419176181</v>
       </c>
       <c r="E31">
-        <v>-85</v>
+        <v>-87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>